<commit_message>
Updated datafile for SAV
</commit_message>
<xml_diff>
--- a/data-raw/Wilcox - SAV Table for SOE Report - David Wilcox.xlsx
+++ b/data-raw/Wilcox - SAV Table for SOE Report - David Wilcox.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwilcox\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Current Projects\Annual Mapping\SOE Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643DBB22-9946-4C5B-ABE5-DE52FEC22DB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA87BEF-6C35-4B9E-BE18-9FEE8D561B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{13C8E3A2-E6FB-475A-AAE8-164943661608}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{13C8E3A2-E6FB-475A-AAE8-164943661608}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,7 +57,7 @@
     <t>Year</t>
   </si>
   <si>
-    <t>SAV Acres in the Chesapeake Bay by VIMS Bay Salinity Zones. See https://www.chesapeakeprogress.com/abundant-life/sav  and https://www.vims.edu/sav  VIMS 10/20/23</t>
+    <t>SAV Acres in the Chesapeake Bay by VIMS Bay Salinity Zones. See https://www.chesapeakeprogress.com/abundant-life/sav  and https://www.vims.edu/sav  VIMS 10/23/24</t>
   </si>
 </sst>
 </file>
@@ -57,7 +68,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +83,540 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="56"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="56"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="56"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="56"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="55">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="30"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="36"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="62"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -89,18 +624,870 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="63"/>
+      </left>
+      <right style="double">
+        <color indexed="63"/>
+      </right>
+      <top style="double">
+        <color indexed="63"/>
+      </top>
+      <bottom style="double">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="30"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="52"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="62"/>
+      </top>
+      <bottom style="double">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="51" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="54" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="51" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="51" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="54" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="51" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="321">
+    <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{0AFE57F7-0DD4-4FD8-AA50-8CDD2920CE29}"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="94" xr:uid="{D5E6F0C9-5CB5-45D1-B780-96B67E56F315}"/>
+    <cellStyle name="20% - Accent1 2 2 2" xfId="253" xr:uid="{93EA8BB2-FD92-4761-840E-2F4D09981A25}"/>
+    <cellStyle name="20% - Accent1 2 3" xfId="217" xr:uid="{747BAA07-5358-4087-8F6D-B86BD6792EAA}"/>
+    <cellStyle name="20% - Accent1 3" xfId="115" xr:uid="{9E195C0F-FE55-4FD7-9311-20CE1246D3AA}"/>
+    <cellStyle name="20% - Accent1 3 2" xfId="270" xr:uid="{A06F8AC7-E0FF-4491-9A5D-3EB43EB6DEBF}"/>
+    <cellStyle name="20% - Accent1 4" xfId="133" xr:uid="{931389AA-652C-48F3-8E59-59317502EC62}"/>
+    <cellStyle name="20% - Accent1 4 2" xfId="286" xr:uid="{8F834C0D-DA1A-446F-BA68-16D7085F3C95}"/>
+    <cellStyle name="20% - Accent1 5" xfId="151" xr:uid="{26383AF7-AAD5-4B5F-A807-B13D2BDB2D90}"/>
+    <cellStyle name="20% - Accent1 5 2" xfId="304" xr:uid="{C2BF00D4-F534-4FB8-9C87-41685AC5B152}"/>
+    <cellStyle name="20% - Accent1 6" xfId="169" xr:uid="{8825D434-3BBA-45DF-ACDD-982E404D0D46}"/>
+    <cellStyle name="20% - Accent1 7" xfId="207" xr:uid="{0A324852-DF54-429F-8B26-ECFDC5E3D156}"/>
+    <cellStyle name="20% - Accent1 8" xfId="3" xr:uid="{7123B1FF-1524-4070-9A01-77740D00E943}"/>
+    <cellStyle name="20% - Accent2 2" xfId="48" xr:uid="{8E4F361A-FD28-44DB-B0B0-D928DDA89BD0}"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="95" xr:uid="{72CC526C-9431-4437-93F1-18ECE01A47F6}"/>
+    <cellStyle name="20% - Accent2 2 2 2" xfId="254" xr:uid="{4646F82C-3743-416E-9A4D-9432D1695A0D}"/>
+    <cellStyle name="20% - Accent2 2 3" xfId="219" xr:uid="{3E736724-5913-41E0-9204-3CFAA47A78AE}"/>
+    <cellStyle name="20% - Accent2 3" xfId="117" xr:uid="{3E31623B-9007-4806-862C-E6CFE14A8DD0}"/>
+    <cellStyle name="20% - Accent2 3 2" xfId="272" xr:uid="{2AF0E12A-4248-4B97-AF54-0D1ED5E10C85}"/>
+    <cellStyle name="20% - Accent2 4" xfId="134" xr:uid="{946C8464-6D86-4870-9146-66B692C5D620}"/>
+    <cellStyle name="20% - Accent2 4 2" xfId="287" xr:uid="{498B0FF8-24C5-45E0-9F30-82D8B8695E5F}"/>
+    <cellStyle name="20% - Accent2 5" xfId="153" xr:uid="{70067BEB-9619-4BDF-9637-505324AE669A}"/>
+    <cellStyle name="20% - Accent2 5 2" xfId="306" xr:uid="{53D836FB-767F-4370-98CE-67FB3D9BD061}"/>
+    <cellStyle name="20% - Accent2 6" xfId="170" xr:uid="{3563E014-8911-44CD-8354-99D598F41EE6}"/>
+    <cellStyle name="20% - Accent2 7" xfId="206" xr:uid="{5D1CAF44-7141-45F2-9A70-FF0227AC2C74}"/>
+    <cellStyle name="20% - Accent2 8" xfId="4" xr:uid="{4AD06AC5-4315-46DD-A560-EF91687D4588}"/>
+    <cellStyle name="20% - Accent3 2" xfId="49" xr:uid="{61A99565-A371-430F-9084-53AB2239085F}"/>
+    <cellStyle name="20% - Accent3 2 2" xfId="96" xr:uid="{A5CBDB69-DB59-4523-871D-AA350FAD4C46}"/>
+    <cellStyle name="20% - Accent3 2 2 2" xfId="255" xr:uid="{650A5DAF-AB71-4B8B-9864-12AF530CF9D8}"/>
+    <cellStyle name="20% - Accent3 2 3" xfId="221" xr:uid="{37697657-1C1C-4595-9D76-FBF5409296E9}"/>
+    <cellStyle name="20% - Accent3 3" xfId="119" xr:uid="{71D80F5B-E2F0-45DF-9341-4B3CDF4B1EEF}"/>
+    <cellStyle name="20% - Accent3 3 2" xfId="274" xr:uid="{328505F9-1308-4056-AF1B-EAFE63CF1448}"/>
+    <cellStyle name="20% - Accent3 4" xfId="135" xr:uid="{8568496A-17F1-44D6-BCAE-A20B787735D0}"/>
+    <cellStyle name="20% - Accent3 4 2" xfId="288" xr:uid="{1DA4FAC5-05AB-47FD-B528-57F15948DF05}"/>
+    <cellStyle name="20% - Accent3 5" xfId="155" xr:uid="{CAC0305C-F816-4207-AE8D-78BEB4C843D6}"/>
+    <cellStyle name="20% - Accent3 5 2" xfId="308" xr:uid="{5C9C51A9-1E6C-4966-8970-5684B19EA407}"/>
+    <cellStyle name="20% - Accent3 6" xfId="171" xr:uid="{0DCD4BD0-45D1-46AD-9A37-56E5821C4156}"/>
+    <cellStyle name="20% - Accent3 7" xfId="168" xr:uid="{BB1D645B-985E-4A36-9E8C-7F5D98F46F77}"/>
+    <cellStyle name="20% - Accent3 8" xfId="5" xr:uid="{B1AE1AB6-C471-4683-A733-08C7657F8072}"/>
+    <cellStyle name="20% - Accent4 2" xfId="50" xr:uid="{365DF0F5-5924-4683-9219-3CD457008CC5}"/>
+    <cellStyle name="20% - Accent4 2 2" xfId="97" xr:uid="{4DAEE891-B3C4-4330-B7ED-9EECDA7826BA}"/>
+    <cellStyle name="20% - Accent4 2 2 2" xfId="256" xr:uid="{9D16311D-A427-4877-9AB1-1DDE5D7780E7}"/>
+    <cellStyle name="20% - Accent4 2 3" xfId="223" xr:uid="{B2A780BC-25E0-4C56-AFF5-A4793AE25ED6}"/>
+    <cellStyle name="20% - Accent4 3" xfId="121" xr:uid="{B6C9004C-DB5F-473B-84A7-F086C7F9B832}"/>
+    <cellStyle name="20% - Accent4 3 2" xfId="276" xr:uid="{229AE6E8-8C5F-4318-B13C-103198E89257}"/>
+    <cellStyle name="20% - Accent4 4" xfId="136" xr:uid="{CF5D44CE-6154-4583-B909-BDE3750A66BF}"/>
+    <cellStyle name="20% - Accent4 4 2" xfId="289" xr:uid="{4EBA96D7-CF64-4ED7-908F-3E6172F17E2B}"/>
+    <cellStyle name="20% - Accent4 5" xfId="157" xr:uid="{689B7321-89C8-445E-9586-8008C17E06C8}"/>
+    <cellStyle name="20% - Accent4 5 2" xfId="310" xr:uid="{E13B91A7-AB09-4B15-9650-A316D6844B53}"/>
+    <cellStyle name="20% - Accent4 6" xfId="172" xr:uid="{6E73206E-A2F1-4039-A4E8-8E4898D4551F}"/>
+    <cellStyle name="20% - Accent4 7" xfId="205" xr:uid="{97D53618-C58E-4020-A9D3-6D483588C561}"/>
+    <cellStyle name="20% - Accent4 8" xfId="6" xr:uid="{BF8B5DF4-F1ED-43AF-B896-9B8C5E416BEC}"/>
+    <cellStyle name="20% - Accent5 2" xfId="51" xr:uid="{4AC74FEC-5002-4EDE-BBA4-41DED5BFD7D7}"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="98" xr:uid="{EF37401F-0016-4803-86D8-C9591635830C}"/>
+    <cellStyle name="20% - Accent5 2 2 2" xfId="257" xr:uid="{4C16B8D0-335F-4F29-ACE4-24DB692ADE0C}"/>
+    <cellStyle name="20% - Accent5 2 3" xfId="225" xr:uid="{AED819E4-1B1C-4D26-BE9A-3ACE5E6EF0E0}"/>
+    <cellStyle name="20% - Accent5 3" xfId="123" xr:uid="{19FAA0E1-0004-4A86-98A1-97DA62EB4C44}"/>
+    <cellStyle name="20% - Accent5 3 2" xfId="278" xr:uid="{B64B42AD-0260-46B9-A4A2-2654B027A43E}"/>
+    <cellStyle name="20% - Accent5 4" xfId="137" xr:uid="{14508C9B-F676-48BE-A259-6A838CE81833}"/>
+    <cellStyle name="20% - Accent5 4 2" xfId="290" xr:uid="{72246AE0-B584-436E-BF6F-723EAADE9C49}"/>
+    <cellStyle name="20% - Accent5 5" xfId="159" xr:uid="{A9FE11FB-E126-4F8A-8AAE-7E01D571BA3A}"/>
+    <cellStyle name="20% - Accent5 5 2" xfId="312" xr:uid="{C1FF3798-7865-4DB1-B8EA-C6595167480D}"/>
+    <cellStyle name="20% - Accent5 6" xfId="173" xr:uid="{5D60FBF8-3B42-4F9E-A77C-1243DD5826F4}"/>
+    <cellStyle name="20% - Accent5 7" xfId="204" xr:uid="{8B3ABFB6-5768-4489-A71E-0081A0C4AC6B}"/>
+    <cellStyle name="20% - Accent5 8" xfId="7" xr:uid="{23361E77-D049-418F-AED7-F85096C2D561}"/>
+    <cellStyle name="20% - Accent6 2" xfId="52" xr:uid="{543F9D11-E2FB-4CEB-9C50-782268AB837B}"/>
+    <cellStyle name="20% - Accent6 2 2" xfId="99" xr:uid="{B4BB029B-0AA6-47F9-86DD-2D2A5F79EDB3}"/>
+    <cellStyle name="20% - Accent6 2 2 2" xfId="258" xr:uid="{9518EB84-76C9-4955-A213-8D3DAB8FB98C}"/>
+    <cellStyle name="20% - Accent6 2 3" xfId="227" xr:uid="{249110A6-BF2C-41F3-AC83-2FCC12E5A64C}"/>
+    <cellStyle name="20% - Accent6 3" xfId="125" xr:uid="{8BD520BF-A485-4DC2-BDA4-7868EAA5B220}"/>
+    <cellStyle name="20% - Accent6 3 2" xfId="280" xr:uid="{2C6C22F0-4F0C-4AC7-A5FC-749BBF9E4818}"/>
+    <cellStyle name="20% - Accent6 4" xfId="138" xr:uid="{584BACCA-29B6-4958-8D97-27D1D66B0D23}"/>
+    <cellStyle name="20% - Accent6 4 2" xfId="291" xr:uid="{A3FF327C-F34A-423C-9318-27499D381AE1}"/>
+    <cellStyle name="20% - Accent6 5" xfId="161" xr:uid="{746CC54E-31D0-4299-B2F5-745C5178947B}"/>
+    <cellStyle name="20% - Accent6 5 2" xfId="314" xr:uid="{408B3264-FC4B-4AED-9AE1-795F065087E7}"/>
+    <cellStyle name="20% - Accent6 6" xfId="174" xr:uid="{C40988F1-4F1A-4FC1-B377-8CF48F11A203}"/>
+    <cellStyle name="20% - Accent6 7" xfId="203" xr:uid="{B69F7297-128B-4FCC-A8ED-BCB638130EAF}"/>
+    <cellStyle name="20% - Accent6 8" xfId="8" xr:uid="{A46FE808-8CD3-4BB3-929C-E707B4F1B4E7}"/>
+    <cellStyle name="40% - Accent1 2" xfId="53" xr:uid="{2A98946B-EF5A-4631-BF99-04D019499AF3}"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="100" xr:uid="{C8D2F36E-D70A-4EEC-B6EA-16CA1323E8FC}"/>
+    <cellStyle name="40% - Accent1 2 2 2" xfId="259" xr:uid="{AC30247D-E05C-4FC3-A7D3-DCB36F6BA684}"/>
+    <cellStyle name="40% - Accent1 2 3" xfId="218" xr:uid="{6702C4C2-FF0C-4632-96C1-904D55A74961}"/>
+    <cellStyle name="40% - Accent1 3" xfId="116" xr:uid="{BFB62A37-D728-41D4-96D7-6659D4C494BE}"/>
+    <cellStyle name="40% - Accent1 3 2" xfId="271" xr:uid="{9CE88FF8-52E1-46C2-BEA4-B6E807FD7D06}"/>
+    <cellStyle name="40% - Accent1 4" xfId="139" xr:uid="{696CCAA3-29D7-4170-8047-0FAF8BFD91C5}"/>
+    <cellStyle name="40% - Accent1 4 2" xfId="292" xr:uid="{B17202CE-FAF4-4E16-B9DD-AF5F982E2E7B}"/>
+    <cellStyle name="40% - Accent1 5" xfId="152" xr:uid="{C44ED655-9CC2-4DEF-B973-13A6D8953D3E}"/>
+    <cellStyle name="40% - Accent1 5 2" xfId="305" xr:uid="{A3CB5DE0-47B9-4C34-9F26-D200134C76B2}"/>
+    <cellStyle name="40% - Accent1 6" xfId="175" xr:uid="{8E23B53E-A118-4F4F-98A1-023DC2B1D9CE}"/>
+    <cellStyle name="40% - Accent1 7" xfId="202" xr:uid="{4E2E5BBE-E451-470B-B775-34F0A47C12E2}"/>
+    <cellStyle name="40% - Accent1 8" xfId="9" xr:uid="{C4CF998C-4F45-402C-A288-CF5FCA7F7270}"/>
+    <cellStyle name="40% - Accent2 2" xfId="54" xr:uid="{D89CFD78-BB3A-4E7B-9FE0-7679C2E73842}"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="101" xr:uid="{D04C2B4B-5F0A-4AD6-B8DB-0270B53621FC}"/>
+    <cellStyle name="40% - Accent2 2 2 2" xfId="260" xr:uid="{0795A318-032A-4C34-8B81-1524F5656E12}"/>
+    <cellStyle name="40% - Accent2 2 3" xfId="220" xr:uid="{3A143475-D316-4EDF-AA20-6BFF514C9969}"/>
+    <cellStyle name="40% - Accent2 3" xfId="118" xr:uid="{38451663-E0D8-4681-B710-6885499F0DE0}"/>
+    <cellStyle name="40% - Accent2 3 2" xfId="273" xr:uid="{6D843FBC-2E08-49C8-B20E-B2C83AA0A504}"/>
+    <cellStyle name="40% - Accent2 4" xfId="140" xr:uid="{515F6A57-A5F8-4944-9930-45F07C109A50}"/>
+    <cellStyle name="40% - Accent2 4 2" xfId="293" xr:uid="{9D4F53AD-F6DD-4436-8724-D5C5FED7856C}"/>
+    <cellStyle name="40% - Accent2 5" xfId="154" xr:uid="{B051D1B3-373C-46BE-BADA-58A43AA67E37}"/>
+    <cellStyle name="40% - Accent2 5 2" xfId="307" xr:uid="{2F48D81C-F7A8-4683-B262-5B11E47F206F}"/>
+    <cellStyle name="40% - Accent2 6" xfId="176" xr:uid="{4DB63ECA-601A-488C-B20E-73E7D976BE9A}"/>
+    <cellStyle name="40% - Accent2 7" xfId="201" xr:uid="{26B78670-88DD-4CC7-BFAF-93BA9BF7C802}"/>
+    <cellStyle name="40% - Accent2 8" xfId="10" xr:uid="{61DA248D-D02D-4E8E-8086-2C1314BEC51C}"/>
+    <cellStyle name="40% - Accent3 2" xfId="55" xr:uid="{C04A495B-7857-48F2-A018-AA4B594DF091}"/>
+    <cellStyle name="40% - Accent3 2 2" xfId="102" xr:uid="{548F850A-3250-40AF-B68A-3FCB05E0F40C}"/>
+    <cellStyle name="40% - Accent3 2 2 2" xfId="261" xr:uid="{2F18A61F-E89B-4A23-995C-901041EB2FBC}"/>
+    <cellStyle name="40% - Accent3 2 3" xfId="222" xr:uid="{7E8823DB-9742-45E4-A9A2-432D1B81451B}"/>
+    <cellStyle name="40% - Accent3 3" xfId="120" xr:uid="{DCCE5FF2-CCB8-4F80-8D44-F5A2B430AC6A}"/>
+    <cellStyle name="40% - Accent3 3 2" xfId="275" xr:uid="{C5AAC708-EED0-47C3-B22C-039418DEF0A7}"/>
+    <cellStyle name="40% - Accent3 4" xfId="141" xr:uid="{F93398DF-BB2E-47C5-89FE-729ED596DE51}"/>
+    <cellStyle name="40% - Accent3 4 2" xfId="294" xr:uid="{7944D979-B3F6-4704-9527-AD0F09B40CE1}"/>
+    <cellStyle name="40% - Accent3 5" xfId="156" xr:uid="{B652E135-9D3C-45B0-8580-3B1844C86DD1}"/>
+    <cellStyle name="40% - Accent3 5 2" xfId="309" xr:uid="{47F6E028-BDFF-4C84-BBFF-1ED2089DDAA0}"/>
+    <cellStyle name="40% - Accent3 6" xfId="177" xr:uid="{2164EF46-8402-42FD-950A-580A4A3C5381}"/>
+    <cellStyle name="40% - Accent3 7" xfId="200" xr:uid="{CB33A687-DA30-4538-A644-A89161378A0F}"/>
+    <cellStyle name="40% - Accent3 8" xfId="11" xr:uid="{88E51138-564E-4E0E-9B03-BEFAC92D84A6}"/>
+    <cellStyle name="40% - Accent4 2" xfId="56" xr:uid="{96106D7B-4E30-47F9-81C2-46873A233375}"/>
+    <cellStyle name="40% - Accent4 2 2" xfId="103" xr:uid="{6DF389A4-7425-42E2-90EE-5B76562CB364}"/>
+    <cellStyle name="40% - Accent4 2 2 2" xfId="262" xr:uid="{59F3DB5B-D8DD-43D3-908A-86CDEF2CC62C}"/>
+    <cellStyle name="40% - Accent4 2 3" xfId="224" xr:uid="{E31D8B8D-DA56-4912-87F1-855A95B7E1FB}"/>
+    <cellStyle name="40% - Accent4 3" xfId="122" xr:uid="{C07A9A4D-FCEC-4EDD-B84E-F8A2B4E568FE}"/>
+    <cellStyle name="40% - Accent4 3 2" xfId="277" xr:uid="{83F8ECCB-C4E2-40D6-868C-F85B0B378350}"/>
+    <cellStyle name="40% - Accent4 4" xfId="142" xr:uid="{1379837C-BA21-42BC-87E1-D68B3D67FB90}"/>
+    <cellStyle name="40% - Accent4 4 2" xfId="295" xr:uid="{71F6F930-A14A-4EF0-89E5-46173CC64934}"/>
+    <cellStyle name="40% - Accent4 5" xfId="158" xr:uid="{C8A3855C-5076-4AAE-B4B3-4007D7CD775A}"/>
+    <cellStyle name="40% - Accent4 5 2" xfId="311" xr:uid="{C1C2A17A-579F-42CF-A720-837947732BBE}"/>
+    <cellStyle name="40% - Accent4 6" xfId="178" xr:uid="{06AD05B3-FCEE-45E3-AA3D-D36CBDEF27C0}"/>
+    <cellStyle name="40% - Accent4 7" xfId="199" xr:uid="{91F4BC3D-9588-4476-9050-1E5CB61DDDA6}"/>
+    <cellStyle name="40% - Accent4 8" xfId="12" xr:uid="{0E0A98AA-66BA-4D1B-9D38-AD0883C33046}"/>
+    <cellStyle name="40% - Accent5 2" xfId="57" xr:uid="{D4B0675E-35A9-4454-B88B-06643D692B74}"/>
+    <cellStyle name="40% - Accent5 2 2" xfId="104" xr:uid="{0B1DFB7A-8B5A-4AE6-B2B2-94ACB128CACF}"/>
+    <cellStyle name="40% - Accent5 2 2 2" xfId="263" xr:uid="{5C45FADB-4533-4195-9360-F5F609E0FA98}"/>
+    <cellStyle name="40% - Accent5 2 3" xfId="226" xr:uid="{EC80403A-4B81-4CE9-8E79-1DEDDED295D9}"/>
+    <cellStyle name="40% - Accent5 3" xfId="124" xr:uid="{71100BE1-81D3-46A9-8C79-0F5A2E88B463}"/>
+    <cellStyle name="40% - Accent5 3 2" xfId="279" xr:uid="{DD0661EE-4D97-48B3-9B7D-1F0A95C3D0EE}"/>
+    <cellStyle name="40% - Accent5 4" xfId="143" xr:uid="{4A810886-363F-4B7B-8684-58E6D28D2975}"/>
+    <cellStyle name="40% - Accent5 4 2" xfId="296" xr:uid="{BED3159D-67A8-43BC-B979-390974C8C5CA}"/>
+    <cellStyle name="40% - Accent5 5" xfId="160" xr:uid="{391E8AAC-5D83-4F2A-A194-D604A539F874}"/>
+    <cellStyle name="40% - Accent5 5 2" xfId="313" xr:uid="{AEF8B952-CE44-42A9-99A7-8481709C288A}"/>
+    <cellStyle name="40% - Accent5 6" xfId="179" xr:uid="{4A55A9C3-12D8-4027-9718-1DC5E8388FC9}"/>
+    <cellStyle name="40% - Accent5 7" xfId="198" xr:uid="{DEDB1075-BD0E-4A58-84C0-2C4725EB80A6}"/>
+    <cellStyle name="40% - Accent5 8" xfId="13" xr:uid="{1F9A46DE-C755-4212-9F37-AB7481767B15}"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{F9E2807E-02E1-4609-A6E4-B3C4CCC83757}"/>
+    <cellStyle name="40% - Accent6 2 2" xfId="105" xr:uid="{39A1566D-D82A-4CD1-9BE7-4923388EC020}"/>
+    <cellStyle name="40% - Accent6 2 2 2" xfId="264" xr:uid="{D2935A69-9E73-4ED1-BE5A-2C093924908A}"/>
+    <cellStyle name="40% - Accent6 2 3" xfId="228" xr:uid="{8835FF45-5096-4BEB-AE5D-A2E0883A2983}"/>
+    <cellStyle name="40% - Accent6 3" xfId="126" xr:uid="{B6F457BD-E8CC-4448-9D44-0F353077DC12}"/>
+    <cellStyle name="40% - Accent6 3 2" xfId="281" xr:uid="{BBC7525C-54BE-40CF-AF8A-1A3DBF3DF7DD}"/>
+    <cellStyle name="40% - Accent6 4" xfId="144" xr:uid="{E156D2EB-CF05-4359-8C66-F9A5E9FF8379}"/>
+    <cellStyle name="40% - Accent6 4 2" xfId="297" xr:uid="{C108CE75-3C5B-4559-BBA7-8317BAA6149C}"/>
+    <cellStyle name="40% - Accent6 5" xfId="162" xr:uid="{3CB9A370-C2CE-4F66-8EDC-95B40D21DDAB}"/>
+    <cellStyle name="40% - Accent6 5 2" xfId="315" xr:uid="{27514F99-7DA7-4BDE-8EB1-8D8FDE7CEBD0}"/>
+    <cellStyle name="40% - Accent6 6" xfId="180" xr:uid="{15C08C99-04A2-4698-AC31-F9E2E0F56E84}"/>
+    <cellStyle name="40% - Accent6 7" xfId="197" xr:uid="{9F699DC6-357D-4E3F-B952-8993596ED449}"/>
+    <cellStyle name="40% - Accent6 8" xfId="14" xr:uid="{1F9E8105-AEC2-4C22-B07D-B7072340EBAB}"/>
+    <cellStyle name="60% - Accent1 2" xfId="59" xr:uid="{ED3F0E96-E573-49D8-8D2E-63A21ACE65F4}"/>
+    <cellStyle name="60% - Accent1 3" xfId="196" xr:uid="{C3B22C5E-E78D-495C-8922-52BB837EEC9C}"/>
+    <cellStyle name="60% - Accent1 4" xfId="15" xr:uid="{EDDDD1C7-F1E5-4B4F-BBF3-DD22884E79E5}"/>
+    <cellStyle name="60% - Accent2 2" xfId="60" xr:uid="{F3232123-7138-4B6D-BEB9-B42ED2E3A5A5}"/>
+    <cellStyle name="60% - Accent2 3" xfId="195" xr:uid="{0EAE4B2F-C568-4E1D-952A-F31E1FD27136}"/>
+    <cellStyle name="60% - Accent2 4" xfId="16" xr:uid="{57B26B8A-85F7-41C1-94B1-18395187D500}"/>
+    <cellStyle name="60% - Accent3 2" xfId="61" xr:uid="{FABF320E-9678-48AF-BD86-C810025FF00F}"/>
+    <cellStyle name="60% - Accent3 3" xfId="194" xr:uid="{D29C188E-2391-4D2E-B180-02F70D91E731}"/>
+    <cellStyle name="60% - Accent3 4" xfId="17" xr:uid="{B7C3E779-8346-4580-9C3C-1443E7A20BAE}"/>
+    <cellStyle name="60% - Accent4 2" xfId="62" xr:uid="{3A5BC8CC-CA35-41D1-81BB-DE31AC1DCEE4}"/>
+    <cellStyle name="60% - Accent4 3" xfId="193" xr:uid="{93E19810-BE10-4EE7-AB32-1B3ECF2B6B94}"/>
+    <cellStyle name="60% - Accent4 4" xfId="18" xr:uid="{1E21059E-A227-4C10-8194-3C0AB17EC8D1}"/>
+    <cellStyle name="60% - Accent5 2" xfId="63" xr:uid="{F9A2FC73-5FA7-4EA6-9EA4-227B5590F1D0}"/>
+    <cellStyle name="60% - Accent5 3" xfId="192" xr:uid="{AC9A2ADD-09FE-4E09-94F1-D6066AA130F6}"/>
+    <cellStyle name="60% - Accent5 4" xfId="19" xr:uid="{EC317058-322E-4A29-AE38-5598068C5849}"/>
+    <cellStyle name="60% - Accent6 2" xfId="64" xr:uid="{0104C5B0-51F5-4805-90B2-BB23D1A56516}"/>
+    <cellStyle name="60% - Accent6 3" xfId="191" xr:uid="{2560323A-BBD5-4FEA-AD2A-8BDBAF9A2E3E}"/>
+    <cellStyle name="60% - Accent6 4" xfId="20" xr:uid="{55956859-C54D-4576-A4E4-CFAB1E16C882}"/>
+    <cellStyle name="Accent1 2" xfId="65" xr:uid="{9B127818-056C-4A8C-887F-35B5B428BAC1}"/>
+    <cellStyle name="Accent1 3" xfId="190" xr:uid="{CE2F43A4-0E85-4D8F-8386-471A632CE5A8}"/>
+    <cellStyle name="Accent1 4" xfId="21" xr:uid="{7DFC3941-E518-469F-ADBC-E58103588A70}"/>
+    <cellStyle name="Accent2 2" xfId="66" xr:uid="{4BAEDFA8-4657-4C7B-97E4-339E3E8AA86F}"/>
+    <cellStyle name="Accent2 3" xfId="189" xr:uid="{BDF645CF-65CA-4520-91B9-5BFF6388D87A}"/>
+    <cellStyle name="Accent2 4" xfId="22" xr:uid="{5C172D0C-FB91-455E-A58B-BEB6724967EB}"/>
+    <cellStyle name="Accent3 2" xfId="67" xr:uid="{F5DDBA77-C155-48E3-AE23-0D1D91753735}"/>
+    <cellStyle name="Accent3 3" xfId="188" xr:uid="{92C3299A-DF0A-4C3C-9817-B07BFEF13636}"/>
+    <cellStyle name="Accent3 4" xfId="23" xr:uid="{74EEE4AF-8F17-44D0-A4F2-94E4980340AC}"/>
+    <cellStyle name="Accent4 2" xfId="68" xr:uid="{2FECBF95-EEA3-4E09-B708-C011C5C9F976}"/>
+    <cellStyle name="Accent4 3" xfId="187" xr:uid="{69BE1101-0458-48B8-ACE6-CB6D0E1EC6A2}"/>
+    <cellStyle name="Accent4 4" xfId="24" xr:uid="{521DBAED-BD37-4389-B0AA-044A50B52612}"/>
+    <cellStyle name="Accent5 2" xfId="69" xr:uid="{783B2402-0AC9-4E87-8001-048E7F4C8819}"/>
+    <cellStyle name="Accent5 3" xfId="186" xr:uid="{B7869B3B-DD86-4D82-B038-BCBBE0370508}"/>
+    <cellStyle name="Accent5 4" xfId="25" xr:uid="{5179F054-4B7F-425A-8A5E-CA9C16846AD4}"/>
+    <cellStyle name="Accent6 2" xfId="70" xr:uid="{3F2EF7C9-08F2-4376-8DC2-7FFE42CCFB77}"/>
+    <cellStyle name="Accent6 3" xfId="185" xr:uid="{0CF066ED-484C-40E8-9544-F2D143A18D8B}"/>
+    <cellStyle name="Accent6 4" xfId="26" xr:uid="{EBA44F58-91F5-4693-B1C2-FA5BA5DBF6F1}"/>
+    <cellStyle name="Bad 2" xfId="71" xr:uid="{C1CDA5D0-5A07-4A90-B985-19F06A69A08B}"/>
+    <cellStyle name="Bad 3" xfId="184" xr:uid="{2F0DF444-9581-4B7B-A380-2DC102A0C5B0}"/>
+    <cellStyle name="Bad 4" xfId="27" xr:uid="{8C71BC2B-6E93-439B-AC4E-C5ABB4E262E3}"/>
+    <cellStyle name="Calculation 2" xfId="72" xr:uid="{2910316D-0F56-4D57-83B9-37192C730C01}"/>
+    <cellStyle name="Calculation 3" xfId="183" xr:uid="{28CD0821-F752-4589-BCA2-8A36DB456F97}"/>
+    <cellStyle name="Calculation 4" xfId="28" xr:uid="{12FADE55-FC89-43F5-9694-4A092935F77E}"/>
+    <cellStyle name="Check Cell 2" xfId="73" xr:uid="{BFF8E784-90FD-474D-B0F9-A34DD717D73A}"/>
+    <cellStyle name="Check Cell 3" xfId="182" xr:uid="{529C0BF6-C6DA-4840-8CF7-DD1866F90134}"/>
+    <cellStyle name="Check Cell 4" xfId="29" xr:uid="{34FAE673-9D50-4B9B-8630-4C09891F567D}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="92" xr:uid="{99BBCB93-18C2-46A0-9983-E5CA2C33B589}"/>
+    <cellStyle name="Comma 2 2" xfId="109" xr:uid="{E3C92265-60D1-453C-A7AA-732A1C8D20A1}"/>
+    <cellStyle name="Comma 2 2 2" xfId="235" xr:uid="{32F56018-C402-4688-B884-189B770D76E2}"/>
+    <cellStyle name="Comma 2 3" xfId="132" xr:uid="{CC0C0BF9-FB1E-4FDD-83FB-0B4F0F4902C8}"/>
+    <cellStyle name="Comma 2 3 2" xfId="285" xr:uid="{75C12863-3ACC-483C-96F2-C6ECF146F42F}"/>
+    <cellStyle name="Comma 2 4" xfId="148" xr:uid="{2DEDEC48-A16F-4B50-AD12-7A7EBC77FF73}"/>
+    <cellStyle name="Comma 2 4 2" xfId="301" xr:uid="{5C01D304-03AE-4ABF-B2B4-B5E6AAEB0AA8}"/>
+    <cellStyle name="Comma 2 5" xfId="211" xr:uid="{3C46B876-0D44-4D71-B4D1-AD69DE6FBC91}"/>
+    <cellStyle name="Comma 3" xfId="74" xr:uid="{C8E0B6BB-F0FF-4387-89C7-4A1E38BADDC8}"/>
+    <cellStyle name="Comma 3 2" xfId="237" xr:uid="{6808D97A-3828-432F-B345-360AF387BD1D}"/>
+    <cellStyle name="Comma 3 3" xfId="213" xr:uid="{70053212-B79B-4DE0-B01D-063A7DCDC8BC}"/>
+    <cellStyle name="Comma 4" xfId="112" xr:uid="{D02F4F2E-4D06-4AEB-9735-CB240F1A9AE9}"/>
+    <cellStyle name="Comma 4 2" xfId="230" xr:uid="{0DB61713-D1ED-424F-9758-29EBBEDC26EF}"/>
+    <cellStyle name="Comma 4 3" xfId="268" xr:uid="{43D51AAA-B90B-4551-8D47-F9A6BE2CC93F}"/>
+    <cellStyle name="Comma 5" xfId="127" xr:uid="{B38476B1-29DC-4574-8BE0-6CDA86EB945F}"/>
+    <cellStyle name="Comma 5 2" xfId="215" xr:uid="{E3617AD5-720F-4AED-B2DF-E173B6131DD1}"/>
+    <cellStyle name="Comma 6" xfId="163" xr:uid="{02B2C519-94C1-46F1-A62D-1B271AF9CB02}"/>
+    <cellStyle name="Comma 6 2" xfId="316" xr:uid="{77FDEAB6-3ACE-4558-BF1A-B47D31A6839C}"/>
+    <cellStyle name="Comma 7" xfId="166" xr:uid="{251A7DB2-7AA2-47EE-8B70-0CDE2B8EABB5}"/>
+    <cellStyle name="Comma 7 2" xfId="319" xr:uid="{EE114242-83CD-43FB-BFBA-B7FFECDC36E6}"/>
+    <cellStyle name="Comma 8" xfId="181" xr:uid="{540310FA-CE0F-4CE4-9B85-C748BA385A7A}"/>
+    <cellStyle name="Comma 9" xfId="30" xr:uid="{E3970894-915A-4A94-9298-244B206A50DF}"/>
+    <cellStyle name="Explanatory Text 2" xfId="75" xr:uid="{59A04BF2-72A0-4F0D-91D8-B34BB10BA2E6}"/>
+    <cellStyle name="Explanatory Text 3" xfId="238" xr:uid="{C8C5DDE4-6379-44E5-A9CC-8EBE6284BD0A}"/>
+    <cellStyle name="Explanatory Text 4" xfId="31" xr:uid="{BE6F6F8C-B788-4098-A749-52E3D15CDEBC}"/>
+    <cellStyle name="Good 2" xfId="76" xr:uid="{2071B077-5F2B-4CF7-9990-30EDE6DFD4D7}"/>
+    <cellStyle name="Good 3" xfId="239" xr:uid="{A2803BBF-946B-4051-AFCC-AA246830032E}"/>
+    <cellStyle name="Good 4" xfId="32" xr:uid="{257247DA-FFD0-492D-B88F-7A8FE7C22070}"/>
+    <cellStyle name="Heading 1 2" xfId="77" xr:uid="{34565D25-50E1-4D0F-903F-BC1AF9CF5B1C}"/>
+    <cellStyle name="Heading 1 3" xfId="240" xr:uid="{7EB37205-66E9-4822-979E-FD597778A118}"/>
+    <cellStyle name="Heading 1 4" xfId="33" xr:uid="{760CB7F9-B1E5-47E7-8727-6F0352745A54}"/>
+    <cellStyle name="Heading 2 2" xfId="78" xr:uid="{592B877E-CE7D-4529-A12F-9024FB8C5DD1}"/>
+    <cellStyle name="Heading 2 3" xfId="241" xr:uid="{FF54F4E9-2898-4404-BB6A-99DB50D28AB6}"/>
+    <cellStyle name="Heading 2 4" xfId="34" xr:uid="{C4E40812-BF2C-4E3C-91CD-30CF24865294}"/>
+    <cellStyle name="Heading 3 2" xfId="79" xr:uid="{27C82191-AE06-46B8-A3A4-540CBDFFB869}"/>
+    <cellStyle name="Heading 3 3" xfId="242" xr:uid="{FA850ACD-A113-41D7-8EA9-339E9461EAF2}"/>
+    <cellStyle name="Heading 3 4" xfId="35" xr:uid="{85BE3CF7-2176-49E5-9E8B-AD99399588FF}"/>
+    <cellStyle name="Heading 4 2" xfId="80" xr:uid="{2C4E6AAE-1A2F-4B6C-92C0-53EA7A11460D}"/>
+    <cellStyle name="Heading 4 3" xfId="243" xr:uid="{1E0E51D9-C9AD-4997-9B35-80BD5C8A4B28}"/>
+    <cellStyle name="Heading 4 4" xfId="36" xr:uid="{F29E80D2-2DE1-4F2B-96F6-5A97F3A473F7}"/>
+    <cellStyle name="Input 2" xfId="81" xr:uid="{3F3AD479-4E91-4DCF-BFF1-1C86058E7CD2}"/>
+    <cellStyle name="Input 3" xfId="244" xr:uid="{0A556D6A-FAD7-48F8-BFD2-EB2E0F53A0BD}"/>
+    <cellStyle name="Input 4" xfId="37" xr:uid="{AD095896-091A-48DC-80A1-6DC18FC8C849}"/>
+    <cellStyle name="Linked Cell 2" xfId="82" xr:uid="{0F0D1013-E304-4DA4-A5A6-4D9CACFFA23F}"/>
+    <cellStyle name="Linked Cell 3" xfId="245" xr:uid="{746E840E-82DB-4281-ACA7-ADEE269D9118}"/>
+    <cellStyle name="Linked Cell 4" xfId="38" xr:uid="{B440D47E-ECDE-4F55-A7E9-9F607D4A3A1D}"/>
+    <cellStyle name="Neutral 2" xfId="83" xr:uid="{21665A45-C890-47AC-B9DD-13536FECC338}"/>
+    <cellStyle name="Neutral 3" xfId="246" xr:uid="{3BB2BD10-20D5-4ACF-9A02-242C8FA29AB6}"/>
+    <cellStyle name="Neutral 4" xfId="39" xr:uid="{135118F9-931F-4A2D-9365-42CAFFDF802E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="2" xr:uid="{F082AAFB-95BA-4392-B654-D861731053B9}"/>
+    <cellStyle name="Normal 2" xfId="45" xr:uid="{1D1E0FDB-8C90-4C92-9B32-50059926523A}"/>
+    <cellStyle name="Normal 2 2" xfId="89" xr:uid="{3EB717F7-ADD4-493A-997B-B9E7A6AC4140}"/>
+    <cellStyle name="Normal 2 2 2" xfId="106" xr:uid="{3F1134D3-C2F9-42F3-A328-EAF04BF439A8}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="265" xr:uid="{E1B54065-AE83-497E-80CC-F37D72324F1B}"/>
+    <cellStyle name="Normal 2 2 3" xfId="232" xr:uid="{00A68CF3-3B9E-491C-B5DF-D0265884C839}"/>
+    <cellStyle name="Normal 2 3" xfId="111" xr:uid="{FA0652C4-2297-4BB2-A078-0BB0D731FDE4}"/>
+    <cellStyle name="Normal 2 3 2" xfId="267" xr:uid="{AD8B9F0D-45ED-4E92-A91F-A67B2238DD2B}"/>
+    <cellStyle name="Normal 2 4" xfId="93" xr:uid="{4E9B7A14-8647-4975-9466-F5C7D145EF75}"/>
+    <cellStyle name="Normal 2 4 2" xfId="252" xr:uid="{1B2B14CB-50DF-432D-A07D-223225B47E1E}"/>
+    <cellStyle name="Normal 2 5" xfId="129" xr:uid="{A8F6AC16-6F5E-404F-BACD-AF3B9FC9EEAA}"/>
+    <cellStyle name="Normal 2 5 2" xfId="282" xr:uid="{B727ED95-115D-483A-8B64-3C757DFA74FE}"/>
+    <cellStyle name="Normal 2 6" xfId="145" xr:uid="{22C9F1CD-23DA-45DE-8F6F-18026B7505FF}"/>
+    <cellStyle name="Normal 2 6 2" xfId="298" xr:uid="{36CE6D80-CC5C-4096-8D19-B3C390F15833}"/>
+    <cellStyle name="Normal 2 7" xfId="208" xr:uid="{9A87E4AD-1DCB-4C7C-BBB4-EAF1EF63913B}"/>
+    <cellStyle name="Normal 3" xfId="91" xr:uid="{C5F2315B-E983-44CB-8395-890105BC035A}"/>
+    <cellStyle name="Normal 3 2" xfId="108" xr:uid="{E83D86F9-D456-4A5D-B93A-F9D83452CF5F}"/>
+    <cellStyle name="Normal 3 2 2" xfId="234" xr:uid="{A3E33C43-DA41-4C1E-A7FB-8B79F41FF94F}"/>
+    <cellStyle name="Normal 3 3" xfId="131" xr:uid="{A3395CAA-66D5-4BC5-85C7-365DB292EFBC}"/>
+    <cellStyle name="Normal 3 3 2" xfId="284" xr:uid="{21C245B9-68CD-450C-B78D-76029AE83499}"/>
+    <cellStyle name="Normal 3 4" xfId="147" xr:uid="{0FDD3426-3F51-4575-A09F-5A0661D88A59}"/>
+    <cellStyle name="Normal 3 4 2" xfId="300" xr:uid="{753642B3-E4B2-4D69-8987-E19B98942402}"/>
+    <cellStyle name="Normal 3 5" xfId="210" xr:uid="{42E87F18-EAB8-4EE3-A7B3-6A5C5EFC6032}"/>
+    <cellStyle name="Normal 4" xfId="46" xr:uid="{A7ECEA8E-F1E9-4AC5-ACFA-C91DBFC89816}"/>
+    <cellStyle name="Normal 4 2" xfId="236" xr:uid="{3751A2D1-40C0-4640-905F-54EB023DF365}"/>
+    <cellStyle name="Normal 4 3" xfId="212" xr:uid="{24E47F88-8DCE-4D3B-8C81-8F8C1784D9F3}"/>
+    <cellStyle name="Normal 5" xfId="110" xr:uid="{D9E0A166-27C8-4A58-BF51-82EF48A8E68B}"/>
+    <cellStyle name="Normal 5 2" xfId="229" xr:uid="{28B9E93C-1098-4C57-88A2-B647B6E5F351}"/>
+    <cellStyle name="Normal 5 3" xfId="266" xr:uid="{D93ADC3D-01B2-4F19-B463-C71D65C41FBC}"/>
+    <cellStyle name="Normal 6" xfId="113" xr:uid="{B92376EE-E160-4EB0-991E-3B8267E65D1D}"/>
+    <cellStyle name="Normal 6 2" xfId="214" xr:uid="{9BE0C9D1-798B-4F89-84E1-600C950B407D}"/>
+    <cellStyle name="Normal 7" xfId="149" xr:uid="{296917B8-CE02-4EB3-BD7C-169650F6868F}"/>
+    <cellStyle name="Normal 7 2" xfId="302" xr:uid="{6BE6F8DF-EA6B-412B-92AE-B105AE48ABAB}"/>
+    <cellStyle name="Normal 8" xfId="165" xr:uid="{C6ADDE95-CB7B-4C4B-A4E3-E7995CD9169D}"/>
+    <cellStyle name="Normal 8 2" xfId="318" xr:uid="{799B66E0-91B9-49D6-8F85-812BE4A9E609}"/>
+    <cellStyle name="Normal 9" xfId="231" xr:uid="{750D08CF-7157-4ED0-A65D-4C51B1121049}"/>
+    <cellStyle name="Note 2" xfId="90" xr:uid="{21309A7C-58AD-4FFA-9AF8-58E03EC3D647}"/>
+    <cellStyle name="Note 2 2" xfId="107" xr:uid="{C0A03BBE-DEA3-43AF-9B6E-FBD34DE5C0C4}"/>
+    <cellStyle name="Note 2 2 2" xfId="233" xr:uid="{3A49BB48-7AFE-4D39-A379-D4DC9937EE51}"/>
+    <cellStyle name="Note 2 3" xfId="130" xr:uid="{11860942-90F8-48F4-9A4F-D1ACE0B0D2AB}"/>
+    <cellStyle name="Note 2 3 2" xfId="283" xr:uid="{964C7252-7DED-4545-B26D-358BE191A2C4}"/>
+    <cellStyle name="Note 2 4" xfId="146" xr:uid="{B37F9B45-5695-452D-B881-E4E3FDEFFFA1}"/>
+    <cellStyle name="Note 2 4 2" xfId="299" xr:uid="{5A85A089-80DF-44D2-942D-FC654105EEA8}"/>
+    <cellStyle name="Note 2 5" xfId="209" xr:uid="{C6850F0F-6E57-4A34-80B2-74883B188AB9}"/>
+    <cellStyle name="Note 3" xfId="114" xr:uid="{02DCBB4A-78FD-40D1-83F0-55237EB82D67}"/>
+    <cellStyle name="Note 3 2" xfId="269" xr:uid="{2BAC37D8-AB1A-4969-8750-9D080F14F928}"/>
+    <cellStyle name="Note 4" xfId="150" xr:uid="{DABB6746-B75A-4FED-A147-7FEB06E6CD0F}"/>
+    <cellStyle name="Note 4 2" xfId="303" xr:uid="{F0B61887-AC21-4CA0-8442-42EFF06B3459}"/>
+    <cellStyle name="Note 5" xfId="247" xr:uid="{5FEE1A65-31BA-4143-BC7A-FFEF6EDB63AA}"/>
+    <cellStyle name="Note 6" xfId="40" xr:uid="{EE91C307-F98A-4529-A580-7E7C854A5F8A}"/>
+    <cellStyle name="Output 2" xfId="84" xr:uid="{0A1D8603-003D-4DC1-9303-909F4C9BF49C}"/>
+    <cellStyle name="Output 3" xfId="248" xr:uid="{16D9A727-E365-4D7C-A662-612282CF16CC}"/>
+    <cellStyle name="Output 4" xfId="41" xr:uid="{89898493-74E6-4DAD-B2B0-BC303D726D82}"/>
+    <cellStyle name="Percent 2" xfId="85" xr:uid="{877E0BE9-9E4A-458E-9D2C-263985A6853A}"/>
+    <cellStyle name="Percent 3" xfId="128" xr:uid="{1DA6D8AD-11B5-40FD-A73F-2ABE8600A811}"/>
+    <cellStyle name="Percent 3 2" xfId="216" xr:uid="{B678C663-083B-4EB9-8CFF-87D377AC3C11}"/>
+    <cellStyle name="Percent 4" xfId="164" xr:uid="{21C07063-5CF8-4277-AFCC-432893B32CD5}"/>
+    <cellStyle name="Percent 4 2" xfId="317" xr:uid="{17330076-BCD8-48E2-9553-D3F6DF045218}"/>
+    <cellStyle name="Percent 5" xfId="320" xr:uid="{A99B0A9B-BC01-445B-BD6C-2B17CA5DD30C}"/>
+    <cellStyle name="Percent 6" xfId="167" xr:uid="{4A2AC087-7B4E-4807-829F-860E75BFB69D}"/>
+    <cellStyle name="Title 2" xfId="86" xr:uid="{AD71A1C2-D022-4661-9CFB-A8152089464F}"/>
+    <cellStyle name="Title 3" xfId="249" xr:uid="{E186D423-ACEC-4AD8-A8A4-6E37933C128B}"/>
+    <cellStyle name="Title 4" xfId="42" xr:uid="{EA8F766F-9BF1-47BB-A987-96848C2D5574}"/>
+    <cellStyle name="Total 2" xfId="87" xr:uid="{925924A1-C49A-4784-988E-F8A9AB2C5A15}"/>
+    <cellStyle name="Total 3" xfId="250" xr:uid="{4A8CD4E6-5209-4DFF-B224-D792344A85BF}"/>
+    <cellStyle name="Total 4" xfId="43" xr:uid="{A6031395-36B8-45BA-A56E-A71DB1F23647}"/>
+    <cellStyle name="Warning Text 2" xfId="88" xr:uid="{FD9CA3BA-7BA6-456D-9F5B-FF4A6658FDD4}"/>
+    <cellStyle name="Warning Text 3" xfId="251" xr:uid="{62516AA1-87C1-407E-9B51-8DA7AAF20782}"/>
+    <cellStyle name="Warning Text 4" xfId="44" xr:uid="{D0294FCC-CB7A-41DC-9D6A-4F6298ADE7A5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,7 +1856,7 @@
                   <c:v>19244.72571967469</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>19185.440190206144</c:v>
+                  <c:v>19411.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -760,7 +2147,7 @@
                   <c:v>8384.0192715271569</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7145.1419896719117</c:v>
+                  <c:v>7175.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1051,7 +2438,7 @@
                   <c:v>24091.100197637355</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>30931.502311361433</c:v>
+                  <c:v>31376.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,7 +2735,7 @@
                   <c:v>16371.420865570204</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>19199.66861381636</c:v>
+                  <c:v>19462.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,7 +3026,7 @@
                   <c:v>68091.266054409411</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76461.753105055846</c:v>
+                  <c:v>77424.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2486,7 +3873,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{8ADBB2B1-E34E-40D2-8665-B301F71719E9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="69" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2497,7 +3884,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8682935" cy="6294783"/>
+    <xdr:ext cx="8677362" cy="6291743"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2527,9 +3914,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2567,7 +3954,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2673,7 +4060,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2815,7 +4202,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2823,10 +4210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC34370-29BA-42C8-B125-C46ECD3E6C9B}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2836,6 +4223,7 @@
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3463,7 +4851,7 @@
         <v>75438.259730999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2015</v>
       </c>
@@ -3483,7 +4871,7 @@
         <v>92314.804271891437</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2016</v>
       </c>
@@ -3503,7 +4891,7 @@
         <v>99618.22066493734</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -3523,7 +4911,7 @@
         <v>104892.87621719918</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -3543,7 +4931,7 @@
         <v>108077.86083382118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2019</v>
       </c>
@@ -3563,7 +4951,7 @@
         <v>66684.118055899802</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -3583,7 +4971,7 @@
         <v>63131.589072218638</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -3603,24 +4991,46 @@
         <v>68091.266054409411</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2022</v>
       </c>
       <c r="B40" s="1">
-        <v>19185.440190206144</v>
+        <v>19411.28</v>
       </c>
       <c r="C40" s="1">
-        <v>7145.1419896719117</v>
+        <v>7175.05</v>
       </c>
       <c r="D40" s="1">
-        <v>30931.502311361433</v>
+        <v>31376.26</v>
       </c>
       <c r="E40" s="1">
-        <v>19199.66861381636</v>
+        <v>19462.32</v>
       </c>
       <c r="F40" s="1">
-        <v>76461.753105055846</v>
+        <v>77424.91</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2023</v>
+      </c>
+      <c r="B41" s="1">
+        <v>19804.150000000001</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3428.71</v>
+      </c>
+      <c r="D41" s="1">
+        <v>37960.67</v>
+      </c>
+      <c r="E41" s="1">
+        <v>21743.31</v>
+      </c>
+      <c r="F41" s="1">
+        <v>82936.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>